<commit_message>
Added some links to creating walkthroughs.
</commit_message>
<xml_diff>
--- a/checking-bayes-filer.xlsx
+++ b/checking-bayes-filer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajcd2020/Documents/Repositories/probabilistic-robotics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D9FBE1B-CCC5-DE41-98B9-CB0D14C66987}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24CE061-4F6A-7C46-93FE-7B6E58E53EB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{E18F49D9-639F-4D4F-B04B-A321A737B091}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>Iteration</t>
   </si>
@@ -94,18 +94,6 @@
   </si>
   <si>
     <t>C0</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>1,3,4</t>
-  </si>
-  <si>
-    <t>2,4</t>
-  </si>
-  <si>
-    <t>3,5,6,7</t>
   </si>
 </sst>
 </file>
@@ -583,34 +571,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.9307400000000004E-4</c:v>
+                  <c:v>6.1739700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4520699999999999E-2</c:v>
+                  <c:v>8.3388799999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6761100000000001E-2</c:v>
+                  <c:v>3.9351799999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23227200000000001</c:v>
+                  <c:v>2.2533399999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6796499999999999E-2</c:v>
+                  <c:v>2.5150700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23732400000000001</c:v>
+                  <c:v>5.83879E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23253399999999999</c:v>
+                  <c:v>6.0151200000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.233318</c:v>
+                  <c:v>1.9701300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.45687E-2</c:v>
+                  <c:v>0.100948</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.1159900000000002E-4</c:v>
+                  <c:v>0.52864800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -899,34 +887,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>5.9725599999999997E-2</c:v>
+                  <c:v>6.2208399999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9725599999999997E-2</c:v>
+                  <c:v>6.2208399999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.49762E-2</c:v>
+                  <c:v>2.0217700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23872299999999999</c:v>
+                  <c:v>0.23017099999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.49762E-2</c:v>
+                  <c:v>2.0217700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23872299999999999</c:v>
+                  <c:v>0.23017099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.49762E-2</c:v>
+                  <c:v>2.0217700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.9725599999999997E-2</c:v>
+                  <c:v>6.2208399999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23872299999999999</c:v>
+                  <c:v>0.23017099999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9725599999999997E-2</c:v>
+                  <c:v>6.2208399999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1215,34 +1203,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.101882</c:v>
+                  <c:v>9.9626400000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.101882</c:v>
+                  <c:v>9.9626400000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.54513E-2</c:v>
+                  <c:v>2.32254E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.59285E-2</c:v>
+                  <c:v>6.6002500000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10170999999999999</c:v>
+                  <c:v>8.3748400000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.59285E-2</c:v>
+                  <c:v>6.6002500000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10170999999999999</c:v>
+                  <c:v>8.3748400000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.4057899999999997E-3</c:v>
+                  <c:v>9.7758399999999992E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.102187</c:v>
+                  <c:v>0.126526</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.406916</c:v>
+                  <c:v>0.34171899999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1531,34 +1519,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.50296399999999997</c:v>
+                  <c:v>0.16608999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.126024</c:v>
+                  <c:v>5.21147E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1482400000000001E-2</c:v>
+                  <c:v>0.19247300000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.14831E-2</c:v>
+                  <c:v>1.4386899999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.0416099999999994E-3</c:v>
+                  <c:v>0.141817</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.125718</c:v>
+                  <c:v>4.2880599999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.0416099999999994E-3</c:v>
+                  <c:v>0.141817</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.14235E-2</c:v>
+                  <c:v>0.15975800000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0422299999999992E-3</c:v>
+                  <c:v>1.1221E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.126779</c:v>
+                  <c:v>7.7442499999999997E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1847,34 +1835,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.162663</c:v>
+                  <c:v>4.6178299999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.64293400000000001</c:v>
+                  <c:v>8.2767400000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0273900000000001E-2</c:v>
+                  <c:v>0.14157400000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0273900000000001E-2</c:v>
+                  <c:v>9.3453300000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0061199999999999E-2</c:v>
+                  <c:v>5.8063099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0437800000000001E-2</c:v>
+                  <c:v>7.0585200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0168500000000003E-2</c:v>
+                  <c:v>0.11294700000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5792800000000002E-3</c:v>
+                  <c:v>0.30735400000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0168500000000003E-2</c:v>
+                  <c:v>7.7530299999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.04399E-2</c:v>
+                  <c:v>9.5468800000000006E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2163,34 +2151,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.3531799999999999E-2</c:v>
+                  <c:v>1.85881E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.36244399999999999</c:v>
+                  <c:v>7.0126900000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35675600000000002</c:v>
+                  <c:v>3.11846E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9473700000000003E-2</c:v>
+                  <c:v>0.192441</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2351599999999999E-2</c:v>
+                  <c:v>3.1630100000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2353000000000001E-2</c:v>
+                  <c:v>8.3463700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.8137199999999997E-3</c:v>
+                  <c:v>2.63206E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2289E-2</c:v>
+                  <c:v>4.6571300000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.8137199999999997E-3</c:v>
+                  <c:v>0.400146</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.9173600000000006E-2</c:v>
+                  <c:v>9.9528400000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2479,34 +2467,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.139233</c:v>
+                  <c:v>4.4687900000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7298499999999998E-2</c:v>
+                  <c:v>1.16037E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14157900000000001</c:v>
+                  <c:v>0.12948299999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55702099999999999</c:v>
+                  <c:v>2.31226E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.4924900000000002E-2</c:v>
+                  <c:v>0.344779</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.4924900000000002E-2</c:v>
+                  <c:v>1.7992299999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.72531E-3</c:v>
+                  <c:v>0.15199799999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2774499999999999E-3</c:v>
+                  <c:v>5.5415100000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.48013E-2</c:v>
+                  <c:v>4.0042099999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.2143199999999998E-3</c:v>
+                  <c:v>0.18087600000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2795,34 +2783,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.7905799999999999E-2</c:v>
+                  <c:v>9.51819E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26660600000000001</c:v>
+                  <c:v>2.3547999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7918E-2</c:v>
+                  <c:v>5.3246500000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.27209299999999997</c:v>
+                  <c:v>6.7632999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.266594</c:v>
+                  <c:v>0.12585199999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6923800000000006E-2</c:v>
+                  <c:v>0.17760799999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6718400000000001E-2</c:v>
+                  <c:v>7.1459700000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1768200000000004E-3</c:v>
+                  <c:v>0.32400800000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4264200000000004E-3</c:v>
+                  <c:v>3.06605E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.6638000000000003E-2</c:v>
+                  <c:v>3.0801499999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3111,34 +3099,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.32336E-2</c:v>
+                  <c:v>5.1206700000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3342800000000003E-3</c:v>
+                  <c:v>0.121031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37173800000000001</c:v>
+                  <c:v>9.1159399999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.3404400000000001E-3</c:v>
+                  <c:v>7.5195499999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37973600000000002</c:v>
+                  <c:v>2.5251300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.2947299999999997E-2</c:v>
+                  <c:v>0.180172</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.3331300000000006E-2</c:v>
+                  <c:v>5.7406600000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.3315300000000001E-2</c:v>
+                  <c:v>3.3247100000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4574200000000001E-3</c:v>
+                  <c:v>0.405194</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.56613E-3</c:v>
+                  <c:v>4.2179500000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9416,7 +9404,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9476,7 +9464,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -9515,10 +9503,10 @@
         <v>14</v>
       </c>
       <c r="O2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -9526,40 +9514,40 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="1">
-        <v>5.9725599999999997E-2</v>
+        <v>6.2208399999999997E-2</v>
       </c>
       <c r="E3" s="1">
-        <v>5.9725599999999997E-2</v>
+        <v>6.2208399999999997E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>1.49762E-2</v>
+        <v>2.0217700000000002E-2</v>
       </c>
       <c r="G3" s="1">
-        <v>0.23872299999999999</v>
+        <v>0.23017099999999999</v>
       </c>
       <c r="H3" s="1">
-        <v>1.49762E-2</v>
+        <v>2.0217700000000002E-2</v>
       </c>
       <c r="I3" s="1">
-        <v>0.23872299999999999</v>
+        <v>0.23017099999999999</v>
       </c>
       <c r="J3" s="1">
-        <v>1.49762E-2</v>
+        <v>2.0217700000000002E-2</v>
       </c>
       <c r="K3" s="1">
-        <v>5.9725599999999997E-2</v>
+        <v>6.2208399999999997E-2</v>
       </c>
       <c r="L3" s="1">
-        <v>0.23872299999999999</v>
+        <v>0.23017099999999999</v>
       </c>
       <c r="M3" s="1">
-        <v>5.9725599999999997E-2</v>
+        <v>6.2208399999999997E-2</v>
       </c>
       <c r="N3" t="s">
         <v>13</v>
@@ -9576,40 +9564,40 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4" s="1">
-        <v>0.101882</v>
+        <v>9.9626400000000004E-2</v>
       </c>
       <c r="E4" s="1">
-        <v>0.101882</v>
+        <v>9.9626400000000004E-2</v>
       </c>
       <c r="F4" s="1">
-        <v>2.54513E-2</v>
+        <v>2.32254E-2</v>
       </c>
       <c r="G4" s="1">
-        <v>2.59285E-2</v>
+        <v>6.6002500000000006E-2</v>
       </c>
       <c r="H4" s="1">
-        <v>0.10170999999999999</v>
+        <v>8.3748400000000001E-2</v>
       </c>
       <c r="I4" s="1">
-        <v>2.59285E-2</v>
+        <v>6.6002500000000006E-2</v>
       </c>
       <c r="J4" s="1">
-        <v>0.10170999999999999</v>
+        <v>8.3748400000000001E-2</v>
       </c>
       <c r="K4" s="1">
-        <v>6.4057899999999997E-3</v>
+        <v>9.7758399999999992E-3</v>
       </c>
       <c r="L4" s="1">
-        <v>0.102187</v>
+        <v>0.126526</v>
       </c>
       <c r="M4" s="1">
-        <v>0.406916</v>
+        <v>0.34171899999999999</v>
       </c>
       <c r="N4" t="s">
         <v>13</v>
@@ -9626,49 +9614,49 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.50296399999999997</v>
+        <v>0.16608999999999999</v>
       </c>
       <c r="E5" s="1">
-        <v>0.126024</v>
+        <v>5.21147E-2</v>
       </c>
       <c r="F5" s="1">
-        <v>3.1482400000000001E-2</v>
+        <v>0.19247300000000001</v>
       </c>
       <c r="G5" s="1">
-        <v>3.14831E-2</v>
+        <v>1.4386899999999999E-2</v>
       </c>
       <c r="H5" s="1">
-        <v>8.0416099999999994E-3</v>
+        <v>0.141817</v>
       </c>
       <c r="I5" s="1">
-        <v>0.125718</v>
+        <v>4.2880599999999998E-2</v>
       </c>
       <c r="J5" s="1">
-        <v>8.0416099999999994E-3</v>
+        <v>0.141817</v>
       </c>
       <c r="K5" s="1">
-        <v>3.14235E-2</v>
+        <v>0.15975800000000001</v>
       </c>
       <c r="L5" s="1">
-        <v>8.0422299999999992E-3</v>
+        <v>1.1221E-2</v>
       </c>
       <c r="M5" s="1">
-        <v>0.126779</v>
+        <v>7.7442499999999997E-2</v>
       </c>
       <c r="N5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
       </c>
       <c r="P5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -9676,43 +9664,43 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
-        <v>0.162663</v>
+        <v>4.6178299999999999E-2</v>
       </c>
       <c r="E6" s="1">
-        <v>0.64293400000000001</v>
+        <v>8.2767400000000005E-2</v>
       </c>
       <c r="F6" s="1">
-        <v>4.0273900000000001E-2</v>
+        <v>0.14157400000000001</v>
       </c>
       <c r="G6" s="1">
-        <v>4.0273900000000001E-2</v>
+        <v>9.3453300000000003E-2</v>
       </c>
       <c r="H6" s="1">
-        <v>1.0061199999999999E-2</v>
+        <v>5.8063099999999999E-2</v>
       </c>
       <c r="I6" s="1">
-        <v>1.0437800000000001E-2</v>
+        <v>7.0585200000000001E-2</v>
       </c>
       <c r="J6" s="1">
-        <v>4.0168500000000003E-2</v>
+        <v>0.11294700000000001</v>
       </c>
       <c r="K6" s="1">
-        <v>2.5792800000000002E-3</v>
+        <v>0.30735400000000002</v>
       </c>
       <c r="L6" s="1">
-        <v>4.0168500000000003E-2</v>
+        <v>7.7530299999999996E-2</v>
       </c>
       <c r="M6" s="1">
-        <v>1.04399E-2</v>
+        <v>9.5468800000000006E-3</v>
       </c>
       <c r="N6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O6" t="b">
         <v>1</v>
@@ -9726,40 +9714,40 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
       </c>
       <c r="D7" s="1">
-        <v>2.3531799999999999E-2</v>
+        <v>1.85881E-2</v>
       </c>
       <c r="E7" s="1">
-        <v>0.36244399999999999</v>
+        <v>7.0126900000000006E-2</v>
       </c>
       <c r="F7" s="1">
-        <v>0.35675600000000002</v>
+        <v>3.11846E-2</v>
       </c>
       <c r="G7" s="1">
-        <v>8.9473700000000003E-2</v>
+        <v>0.192441</v>
       </c>
       <c r="H7" s="1">
-        <v>2.2351599999999999E-2</v>
+        <v>3.1630100000000001E-2</v>
       </c>
       <c r="I7" s="1">
-        <v>2.2353000000000001E-2</v>
+        <v>8.3463700000000002E-2</v>
       </c>
       <c r="J7" s="1">
-        <v>5.8137199999999997E-3</v>
+        <v>2.63206E-2</v>
       </c>
       <c r="K7" s="1">
-        <v>2.2289E-2</v>
+        <v>4.6571300000000003E-2</v>
       </c>
       <c r="L7" s="1">
-        <v>5.8137199999999997E-3</v>
+        <v>0.400146</v>
       </c>
       <c r="M7" s="1">
-        <v>8.9173600000000006E-2</v>
+        <v>9.9528400000000003E-2</v>
       </c>
       <c r="N7" t="s">
         <v>13</v>
@@ -9768,7 +9756,7 @@
         <v>1</v>
       </c>
       <c r="P7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -9776,43 +9764,43 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
-        <v>0.139233</v>
+        <v>4.4687900000000003E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>3.7298499999999998E-2</v>
+        <v>1.16037E-2</v>
       </c>
       <c r="F8" s="1">
-        <v>0.14157900000000001</v>
+        <v>0.12948299999999999</v>
       </c>
       <c r="G8" s="1">
-        <v>0.55702099999999999</v>
+        <v>2.31226E-2</v>
       </c>
       <c r="H8" s="1">
-        <v>3.4924900000000002E-2</v>
+        <v>0.344779</v>
       </c>
       <c r="I8" s="1">
-        <v>3.4924900000000002E-2</v>
+        <v>1.7992299999999999E-2</v>
       </c>
       <c r="J8" s="1">
-        <v>8.72531E-3</v>
+        <v>0.15199799999999999</v>
       </c>
       <c r="K8" s="1">
-        <v>2.2774499999999999E-3</v>
+        <v>5.5415100000000002E-2</v>
       </c>
       <c r="L8" s="1">
-        <v>3.48013E-2</v>
+        <v>4.0042099999999997E-2</v>
       </c>
       <c r="M8" s="1">
-        <v>9.2143199999999998E-3</v>
+        <v>0.18087600000000001</v>
       </c>
       <c r="N8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O8" t="b">
         <v>1</v>
@@ -9828,47 +9816,47 @@
       <c r="B9">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>21</v>
+      <c r="C9">
+        <v>7</v>
       </c>
       <c r="D9" s="1">
-        <v>1.7905799999999999E-2</v>
+        <v>9.51819E-2</v>
       </c>
       <c r="E9" s="1">
-        <v>0.26660600000000001</v>
+        <v>2.3547999999999999E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>1.7918E-2</v>
+        <v>5.3246500000000002E-2</v>
       </c>
       <c r="G9" s="1">
-        <v>0.27209299999999997</v>
+        <v>6.7632999999999999E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>0.266594</v>
+        <v>0.12585199999999999</v>
       </c>
       <c r="I9" s="1">
-        <v>6.6923800000000006E-2</v>
+        <v>0.17760799999999999</v>
       </c>
       <c r="J9" s="1">
-        <v>1.6718400000000001E-2</v>
+        <v>7.1459700000000001E-2</v>
       </c>
       <c r="K9" s="1">
-        <v>4.1768200000000004E-3</v>
+        <v>0.32400800000000002</v>
       </c>
       <c r="L9" s="1">
-        <v>4.4264200000000004E-3</v>
+        <v>3.06605E-2</v>
       </c>
       <c r="M9" s="1">
-        <v>6.6638000000000003E-2</v>
+        <v>3.0801499999999999E-2</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="O9" t="b">
+        <v>0</v>
+      </c>
+      <c r="P9" t="b">
         <v>1</v>
-      </c>
-      <c r="P9" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -9876,46 +9864,46 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
       </c>
       <c r="D10" s="1">
-        <v>2.32336E-2</v>
+        <v>5.1206700000000001E-2</v>
       </c>
       <c r="E10" s="1">
-        <v>6.3342800000000003E-3</v>
+        <v>0.121031</v>
       </c>
       <c r="F10" s="1">
-        <v>0.37173800000000001</v>
+        <v>9.1159399999999995E-3</v>
       </c>
       <c r="G10" s="1">
-        <v>6.3404400000000001E-3</v>
+        <v>7.5195499999999998E-2</v>
       </c>
       <c r="H10" s="1">
-        <v>0.37973600000000002</v>
+        <v>2.5251300000000001E-2</v>
       </c>
       <c r="I10" s="1">
-        <v>9.2947299999999997E-2</v>
+        <v>0.180172</v>
       </c>
       <c r="J10" s="1">
-        <v>9.3331300000000006E-2</v>
+        <v>5.7406600000000002E-2</v>
       </c>
       <c r="K10" s="1">
-        <v>2.3315300000000001E-2</v>
+        <v>3.3247100000000002E-2</v>
       </c>
       <c r="L10" s="1">
-        <v>1.4574200000000001E-3</v>
+        <v>0.405194</v>
       </c>
       <c r="M10" s="1">
-        <v>1.56613E-3</v>
+        <v>4.2179500000000002E-2</v>
       </c>
       <c r="N10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" t="b">
         <v>0</v>
@@ -9926,43 +9914,43 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
       </c>
       <c r="D11" s="1">
-        <v>9.9307400000000004E-4</v>
+        <v>6.1739700000000002E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>1.4520699999999999E-2</v>
+        <v>8.3388799999999999E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>1.6761100000000001E-2</v>
+        <v>3.9351799999999999E-2</v>
       </c>
       <c r="G11" s="1">
-        <v>0.23227200000000001</v>
+        <v>2.2533399999999999E-2</v>
       </c>
       <c r="H11" s="1">
-        <v>1.6796499999999999E-2</v>
+        <v>2.5150700000000002E-2</v>
       </c>
       <c r="I11" s="1">
-        <v>0.23732400000000001</v>
+        <v>5.83879E-2</v>
       </c>
       <c r="J11" s="1">
-        <v>0.23253399999999999</v>
+        <v>6.0151200000000002E-2</v>
       </c>
       <c r="K11" s="1">
-        <v>0.233318</v>
+        <v>1.9701300000000001E-2</v>
       </c>
       <c r="L11" s="1">
-        <v>1.45687E-2</v>
+        <v>0.100948</v>
       </c>
       <c r="M11" s="1">
-        <v>9.1159900000000002E-4</v>
+        <v>0.52864800000000001</v>
       </c>
       <c r="N11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O11" t="b">
         <v>1</v>

</xml_diff>